<commit_message>
guardando datos antes de injertar datos reales
</commit_message>
<xml_diff>
--- a/Basededatos/postab.xlsx
+++ b/Basededatos/postab.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luzdelsurlds-my.sharepoint.com/personal/roquispec_luzdelsur_com_pe/Documents/Documentos/Estudios de Ingreso/ProyectoRyD_V2/Basededatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{493DCDF4-5E78-457F-A8AB-BED55203E83B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C12A02B9-2994-40D8-958F-E0E93916ED7B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E4B241D-1EF2-4D27-A194-AAB4BA4769B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="7890" xr2:uid="{AF7EA517-A4E3-4372-ACCA-B8037A5E3173}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>SUBESTACION</t>
   </si>
@@ -124,6 +125,9 @@
   </si>
   <si>
     <t>Santa Rosa Nueva</t>
+  </si>
+  <si>
+    <t>POT. INSTALADA</t>
   </si>
 </sst>
 </file>
@@ -276,7 +280,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -352,6 +356,39 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Tahoma"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -394,7 +431,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -407,8 +444,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -506,13 +541,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FDCEECC-5DC3-468D-BEEA-1359675B3BD7}" name="Tabla1" displayName="Tabla1" ref="A1:D19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D19" xr:uid="{9D6F52CC-6266-4B79-9BD8-86ABC06C0811}"/>
-  <sortState ref="A2:B19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FDCEECC-5DC3-468D-BEEA-1359675B3BD7}" name="Tabla1" displayName="Tabla1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E19" xr:uid="{9D6F52CC-6266-4B79-9BD8-86ABC06C0811}"/>
+  <sortState ref="A2:C19">
     <sortCondition ref="A2:A19"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{22615138-724C-48A8-A943-DF3C1FCCD02E}" name="SUBESTACION" dataDxfId="3"/>
+  <tableColumns count="5">
+    <tableColumn id="2" xr3:uid="{22615138-724C-48A8-A943-DF3C1FCCD02E}" name="SUBESTACION" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{C7556C80-0339-427F-A77F-F7A747DC3CD9}" name="POT. INSTALADA" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{438DB061-8B09-4E4A-8B29-8309D102586B}" name="CIRCUITO" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{BE9EB36B-4B01-45C4-8DA4-862EC7D10D13}" name="POS. TAP" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{380C60D0-354E-41C1-94CB-3D43217926B1}" name="TENSION TAP" dataDxfId="0"/>
@@ -818,284 +854,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F43FCAD-666D-401B-B423-233BDB9A09F2}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="5">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="7">
         <v>65.344999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="5">
+        <f>85*3</f>
+        <v>255</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="5">
+        <v>120</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="5">
+        <v>180</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="5">
+        <v>180</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>65.344999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="7">
         <v>65.344999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="5">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="5">
+        <v>120</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="5">
+        <v>50</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="5">
+        <v>50</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="5">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="7">
+      <c r="E14" s="7">
         <v>65.344999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="5">
+        <v>180</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="5">
+        <v>180</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="5">
+        <v>50</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="5">
+        <v>120</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="5">
+        <v>120</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1328,13 +1417,13 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0643612D-F627-4166-BCC1-0961930C51AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="a1cc19d0-e28e-4f1b-b120-4e42c2fee203"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>

</xml_diff>